<commit_message>
coba menambahkan pesan error :)
</commit_message>
<xml_diff>
--- a/Error Bank.xlsx
+++ b/Error Bank.xlsx
@@ -547,7 +547,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -635,6 +635,30 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -643,33 +667,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -948,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1318,6 +1315,9 @@
       </c>
     </row>
     <row r="20" spans="2:7">
+      <c r="B20" s="16">
+        <v>17</v>
+      </c>
       <c r="C20" s="16" t="s">
         <v>110</v>
       </c>
@@ -1330,7 +1330,7 @@
       <c r="F20" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="40">
+      <c r="G20" s="20">
         <v>43559</v>
       </c>
     </row>
@@ -1374,34 +1374,34 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:7" ht="14.45" customHeight="1">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="35" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B3" s="33"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="39"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="36"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="2">
@@ -1504,40 +1504,40 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="30">
+      <c r="B9" s="38">
         <v>6</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="37">
         <v>43368</v>
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="30"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="29"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="37"/>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="29"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="37"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="2">
@@ -1638,17 +1638,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
     <mergeCell ref="G9:G11"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="F9:F11"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>

</xml_diff>

<commit_message>
coba no 22 ni :)
</commit_message>
<xml_diff>
--- a/Error Bank.xlsx
+++ b/Error Bank.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bootcamp\Errors-Bank-Bootcamp-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\Errors-Bank-Bootcamp-master (5)\Errors-Bank-Bootcamp-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Java" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="121">
   <si>
     <t>No</t>
   </si>
@@ -353,16 +353,37 @@
     <t>Delete project layer yang hilang/tidak bisa diload pada project anda melalui Visual Studio 2015. Buka tempat penyimpanan file document project Microservice anda, Misalnya : Document/Visual Studio 2015/Backup Project/"Your Project Name". Copy original file project yang hilang, paste, rename, replace sesuai dengan nama project anda yang tidak bisa diload pada lokasi folder layer project tersebut. Buka kembali Visual Studio 2015 anda, kemudian klik kanan pada Solution Project lalu add Existing Project, lalu add Project file yang baru saja anda copy tadi. Jangan lupa untuk clean dan rebuild file anda kemudian restart Visual Studio anda.</t>
   </si>
   <si>
-    <t>coba git</t>
-  </si>
-  <si>
-    <t>coba aja</t>
-  </si>
-  <si>
-    <t>nanti dihapus</t>
-  </si>
-  <si>
-    <t>Freditya</t>
+    <t>coba</t>
+  </si>
+  <si>
+    <t>adeocaremiwowow</t>
+  </si>
+  <si>
+    <t>baru nih</t>
+  </si>
+  <si>
+    <t>Rahmad</t>
+  </si>
+  <si>
+    <t>Ini baru juga</t>
+  </si>
+  <si>
+    <t>ini ke 20</t>
+  </si>
+  <si>
+    <t>khulqi</t>
+  </si>
+  <si>
+    <t>coba ke 21</t>
+  </si>
+  <si>
+    <t>Oka</t>
+  </si>
+  <si>
+    <t>ke 22 ini</t>
+  </si>
+  <si>
+    <t>fred</t>
   </si>
 </sst>
 </file>
@@ -547,13 +568,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -569,71 +587,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -657,15 +663,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -943,395 +940,439 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G20"/>
+  <dimension ref="B1:G25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="4.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="94.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="126.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="47.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="4.140625" customWidth="1"/>
+    <col min="3" max="3" width="94.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="126.42578125" customWidth="1"/>
+    <col min="6" max="6" width="47.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:7" ht="14.45" customHeight="1">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B3" s="22"/>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="28"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="14">
+      <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="14">
+      <c r="B5" s="7">
         <v>2</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="8">
         <v>43336</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="16">
+      <c r="B6" s="7">
         <v>3</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="16">
+      <c r="B7" s="7">
         <v>4</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="9">
         <v>43333</v>
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="16">
+      <c r="B8" s="7">
         <v>5</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="9">
         <v>43334</v>
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="16">
+      <c r="B9" s="7">
         <v>6</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="16">
+      <c r="B10" s="7">
         <v>7</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="16">
+      <c r="B11" s="7">
         <v>8</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="16">
+      <c r="B12" s="7">
         <v>9</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="16">
+      <c r="B13" s="7">
         <v>10</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="16">
+      <c r="B14" s="7">
         <v>11</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="16">
+      <c r="B15" s="7">
         <v>12</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="8">
         <v>43352</v>
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="16">
+      <c r="B16" s="7">
         <v>13</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="8">
         <v>43357</v>
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="16">
+      <c r="B17" s="7">
         <v>14</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="8">
         <v>43368</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="16">
+      <c r="B18" s="7">
         <v>15</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="8">
         <v>43370</v>
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="16">
+      <c r="B19" s="7">
         <v>16</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="8">
         <v>43467</v>
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="16">
+      <c r="B20" s="7">
         <v>17</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E20" s="16" t="s">
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="7">
+        <v>18</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F21" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="20">
-        <v>43559</v>
+      <c r="G21" s="12">
+        <v>43557</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="7">
+        <v>19</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="7">
+        <v>20</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="7">
+        <v>21</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="7">
+        <v>22</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1360,295 +1401,295 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="6" style="2" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="51" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="6" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="51" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:7" ht="14.45" customHeight="1">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="33" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="30" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B3" s="30"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="36"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="60">
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>43361</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="45">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>43361</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="90">
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>76240</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="135">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>5</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>43368</v>
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="38">
+      <c r="B9" s="22">
         <v>6</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="21">
         <v>43368</v>
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="37"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="37"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>7</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="4">
         <v>43410</v>
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>8</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="4">
         <v>43410</v>
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="10">
+      <c r="B15" s="1">
         <v>9</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="4">
         <v>43293</v>
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="11">
+      <c r="B16" s="1">
         <v>10</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>11</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="4">
         <v>43587</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
     <mergeCell ref="G9:G11"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="F9:F11"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>

</xml_diff>

<commit_message>
tambah bank error by erik
</commit_message>
<xml_diff>
--- a/Error Bank.xlsx
+++ b/Error Bank.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\metrodata\Errors-Bank-Bootcamp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA70DE6E-0DC8-45C0-88BE-33CA88FAD2AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Java" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="129">
   <si>
     <t>No</t>
   </si>
@@ -391,12 +397,24 @@
   </si>
   <si>
     <t>Rizka Nur Fazri</t>
+  </si>
+  <si>
+    <t>site can'be reached 127.0.0.1</t>
+  </si>
+  <si>
+    <t>tidak bisa mengakses oracle yang ada/muncul can't be reached</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ke windows-&gt; services -&gt; OracleServicesXE dan OracleXETNSListener -&gt; restart </t>
+  </si>
+  <si>
+    <t>erick cahya suhanda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -575,7 +593,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -624,6 +642,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -648,6 +669,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -670,15 +700,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -955,7 +976,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G25"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
@@ -976,34 +997,34 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:7" ht="14.45" customHeight="1">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="23" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B3" s="17"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="23"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="7">
@@ -1405,14 +1426,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:G19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1431,34 +1452,34 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:7" ht="14.45" customHeight="1">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="34" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B3" s="25"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="31"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="1">
@@ -1561,40 +1582,40 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="33">
+      <c r="B9" s="26">
         <v>6</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="25">
         <v>43368</v>
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="33"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="32"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="25"/>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="32"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="1">
@@ -1713,19 +1734,39 @@
         <v>43557</v>
       </c>
     </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="1">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" s="16">
+        <v>43562</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
     <mergeCell ref="G9:G11"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="F9:F11"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>

</xml_diff>

<commit_message>
<ini error baru materi ORM hibernate>
</commit_message>
<xml_diff>
--- a/Error Bank.xlsx
+++ b/Error Bank.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\metrodata\Errors-Bank-Bootcamp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofia\Documents\Error-Bank-bootcamp25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA70DE6E-0DC8-45C0-88BE-33CA88FAD2AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Java" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="123">
   <si>
     <t>No</t>
   </si>
@@ -354,39 +353,6 @@
     <t>Delete project layer yang hilang/tidak bisa diload pada project anda melalui Visual Studio 2015. Buka tempat penyimpanan file document project Microservice anda, Misalnya : Document/Visual Studio 2015/Backup Project/"Your Project Name". Copy original file project yang hilang, paste, rename, replace sesuai dengan nama project anda yang tidak bisa diload pada lokasi folder layer project tersebut. Buka kembali Visual Studio 2015 anda, kemudian klik kanan pada Solution Project lalu add Existing Project, lalu add Project file yang baru saja anda copy tadi. Jangan lupa untuk clean dan rebuild file anda kemudian restart Visual Studio anda.</t>
   </si>
   <si>
-    <t>coba</t>
-  </si>
-  <si>
-    <t>adeocaremiwowow</t>
-  </si>
-  <si>
-    <t>baru nih</t>
-  </si>
-  <si>
-    <t>Rahmad</t>
-  </si>
-  <si>
-    <t>Ini baru juga</t>
-  </si>
-  <si>
-    <t>ini ke 20</t>
-  </si>
-  <si>
-    <t>khulqi</t>
-  </si>
-  <si>
-    <t>coba ke 21</t>
-  </si>
-  <si>
-    <t>Oka</t>
-  </si>
-  <si>
-    <t>ke 22 ini</t>
-  </si>
-  <si>
-    <t>fred</t>
-  </si>
-  <si>
     <t>An unhandled exception of type 'System.Data.Entity.Core.MetadataException' occurred in EntityFramework.dll Additional information: Unable to load the specified metadata resource.</t>
   </si>
   <si>
@@ -409,12 +375,27 @@
   </si>
   <si>
     <t>erick cahya suhanda</t>
+  </si>
+  <si>
+    <t>not-null property references a null or transient value : models.Job.jobTitle</t>
+  </si>
+  <si>
+    <t>di model job.java kolom JOB_TITLE optional = false</t>
+  </si>
+  <si>
+    <t>ubah status optional di model job.java menjadi "true"</t>
+  </si>
+  <si>
+    <t>Rahmad Subekti</t>
+  </si>
+  <si>
+    <t>14/05/19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -669,6 +650,30 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -676,30 +681,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -976,18 +957,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:G25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="4.140625" customWidth="1"/>
     <col min="3" max="3" width="94.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" customWidth="1"/>
     <col min="5" max="5" width="126.42578125" customWidth="1"/>
     <col min="6" max="6" width="47.28515625" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
@@ -1351,65 +1332,59 @@
         <v>17</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>111</v>
+        <v>119</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="2:7">
       <c r="B21" s="7">
         <v>18</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G21" s="12">
-        <v>43557</v>
-      </c>
+      <c r="C21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="7">
         <v>19</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>114</v>
-      </c>
+      <c r="C22" s="7"/>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="7">
         <v>20</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>116</v>
-      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="7">
         <v>21</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>118</v>
-      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="7">
         <v>22</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>120</v>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="7">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1426,14 +1401,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1452,34 +1427,34 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:7" ht="14.45" customHeight="1">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="31" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B3" s="29"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="35"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="1">
@@ -1582,40 +1557,40 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="26">
+      <c r="B9" s="34">
         <v>6</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="33">
         <v>43368</v>
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="25"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="25"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="33"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="1">
@@ -1719,16 +1694,16 @@
         <v>12</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="G18" s="13">
         <v>43557</v>
@@ -1739,16 +1714,16 @@
         <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="G19" s="16">
         <v>43562</v>
@@ -1756,17 +1731,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
     <mergeCell ref="G9:G11"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="F9:F11"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>

</xml_diff>

<commit_message>
adding new error on .Net
</commit_message>
<xml_diff>
--- a/Error Bank.xlsx
+++ b/Error Bank.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofia\Documents\Error-Bank-bootcamp25\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NaufalAj\Documents\Git\Errors-Bank-Bootcamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Java" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="126">
   <si>
     <t>No</t>
   </si>
@@ -390,18 +390,34 @@
   </si>
   <si>
     <t>14/05/19</t>
+  </si>
+  <si>
+    <t>Multiple types were found that match the controller named 'Home'</t>
+  </si>
+  <si>
+    <t>terdapat controller Home yang lebih dari 1</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/7842293/multiple-types-were-found-that-match-the-controller-named-home</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -425,6 +441,20 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -569,122 +599,138 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -960,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -978,412 +1024,412 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:7" ht="14.45" customHeight="1">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B3" s="18"/>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="24"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>2</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>43336</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>4</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>43333</v>
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>43334</v>
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>6</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>7</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>8</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>9</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>10</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>11</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>12</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>43352</v>
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>13</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>43357</v>
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>14</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>43368</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>15</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>43370</v>
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>16</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>43467</v>
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>17</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>18</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="12"/>
+      <c r="C21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>19</v>
       </c>
-      <c r="C22" s="7"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>20</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <v>21</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <v>22</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <v>23</v>
       </c>
     </row>
@@ -1402,22 +1448,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G19"/>
+  <dimension ref="B1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="1"/>
     <col min="2" max="2" width="6" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="95.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="82" style="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" style="1" customWidth="1"/>
@@ -1427,46 +1473,46 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:7" ht="14.45" customHeight="1">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="33" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B3" s="26"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1476,91 +1522,91 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="60">
+    <row r="5" spans="2:7">
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="36" t="s">
         <v>64</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>43361</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="45">
+    <row r="6" spans="2:7">
       <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="13">
         <v>43361</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="90">
+    <row r="7" spans="2:7" ht="45">
       <c r="B7" s="1">
         <v>4</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="13">
         <v>76240</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="135">
+    <row r="8" spans="2:7" ht="75">
       <c r="B8" s="1">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="13">
         <v>43368</v>
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="34">
+      <c r="B9" s="25">
         <v>6</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="26" t="s">
         <v>83</v>
       </c>
       <c r="D9" s="35" t="s">
@@ -1569,46 +1615,53 @@
       <c r="E9" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="24">
         <v>43368</v>
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="35"/>
       <c r="E10" s="35"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="33"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="24"/>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="35"/>
       <c r="E11" s="35"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="33"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="C12" s="15"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="1">
         <v>7</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="13">
         <v>43410</v>
       </c>
     </row>
@@ -1616,90 +1669,91 @@
       <c r="B14" s="1">
         <v>8</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="13">
         <v>43410</v>
       </c>
     </row>
-    <row r="15" spans="2:7">
+    <row r="15" spans="2:7" ht="30">
       <c r="B15" s="1">
         <v>9</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="13">
         <v>43293</v>
       </c>
     </row>
-    <row r="16" spans="2:7">
+    <row r="16" spans="2:7" ht="30">
       <c r="B16" s="1">
         <v>10</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="14" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" ht="30">
       <c r="B17" s="1">
         <v>11</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="13">
         <v>43587</v>
       </c>
     </row>
-    <row r="18" spans="2:7" s="14" customFormat="1" ht="90">
-      <c r="B18" s="14">
+    <row r="18" spans="2:7" s="12" customFormat="1" ht="30">
+      <c r="B18" s="12">
         <v>12</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="6" t="s">
         <v>112</v>
       </c>
       <c r="F18" s="14" t="s">
@@ -1713,36 +1767,61 @@
       <c r="B19" s="1">
         <v>13</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G19" s="13">
         <v>43562</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="1">
+        <v>14</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="13">
+        <v>43655</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
     <mergeCell ref="G9:G11"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="F9:F11"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C20" r:id="rId1" display="https://stackoverflow.com/questions/7842293/multiple-types-were-found-that-match-the-controller-named-home"/>
+    <hyperlink ref="E20" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>